<commit_message>
adding fob, weight summary extractor
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/JF.xlsx
+++ b/invoice_gen/TEMPLATE/JF.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" windowWidth="27945" windowHeight="12180" tabRatio="600" firstSheet="0" activeTab="2" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Contract" sheetId="1" state="visible" r:id="rId1"/>
@@ -21,14 +21,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="165" formatCode="###0;###0"/>
     <numFmt numFmtId="166" formatCode="#,##0.00;[Red]#,##0.00"/>
     <numFmt numFmtId="167" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="168" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="53">
+  <fonts count="34">
     <font>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -236,156 +235,12 @@
       <sz val="16"/>
     </font>
     <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF0000FF"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF800080"/>
-      <sz val="11"/>
-      <u val="single"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FFFF0000"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="18"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <i val="1"/>
-      <color rgb="FF7F7F7F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="15"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="13"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <b val="1"/>
-      <color theme="3"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF3F3F76"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FF3F3F3F"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color rgb="FFFFFFFF"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FFFA7D00"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <b val="1"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF006100"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF9C0006"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color rgb="FF9C6500"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color theme="0"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <name val="Arial"/>
       <charset val="134"/>
       <sz val="10"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -404,194 +259,8 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="20">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -692,104 +361,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -819,153 +390,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="50">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="17" fillId="0" borderId="0"/>
     <xf numFmtId="167" fontId="17" fillId="0" borderId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="17" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="17" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="17" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="9" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="10" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="0" borderId="10" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="11" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="41" fillId="5" borderId="12" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="42" fillId="6" borderId="13" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="43" fillId="6" borderId="12" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="44" fillId="7" borderId="14" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="45" fillId="0" borderId="15" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="46" fillId="0" borderId="16" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="47" fillId="8" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="48" fillId="9" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="49" fillId="10" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="11" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="12" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="13" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="14" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="15" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="16" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="17" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="18" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="19" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="20" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="21" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="22" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="23" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="24" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="25" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="26" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="27" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="28" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="29" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="30" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="31" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="32" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="51" fillId="33" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="34" borderId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="132">
+  <cellXfs count="146">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
@@ -975,23 +408,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -1047,8 +466,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1064,7 +481,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1088,9 +504,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1221,90 +634,148 @@
     <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="29" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="4" fontId="29" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="28" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="30" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="3">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="31" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="164" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="29" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="4" fontId="29" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="28" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="30" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="49">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="4" fontId="31" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="2">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="165" fontId="28" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1315,57 +786,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="50">
+  <cellStyles count="4">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
-    <cellStyle name="Percent" xfId="3" builtinId="5"/>
-    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
-    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
-    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
-    <cellStyle name="Note" xfId="8" builtinId="10"/>
-    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
-    <cellStyle name="Title" xfId="10" builtinId="15"/>
-    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
-    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
-    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
-    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
-    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
-    <cellStyle name="Input" xfId="16" builtinId="20"/>
-    <cellStyle name="Output" xfId="17" builtinId="21"/>
-    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
-    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
-    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
-    <cellStyle name="Total" xfId="21" builtinId="25"/>
-    <cellStyle name="Good" xfId="22" builtinId="26"/>
-    <cellStyle name="Bad" xfId="23" builtinId="27"/>
-    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
-    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
-    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
-    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
-    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
-    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
-    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
-    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
-    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
-    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
-    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
-    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
-    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
-    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
-    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
-    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
-    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
-    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
-    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
-    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
-    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
-    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
-    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
-    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
-    <cellStyle name="Normal_SAMPEL " xfId="49"/>
+    <cellStyle name="Normal_SAMPEL " xfId="3"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -2065,6 +1490,7 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
@@ -2076,307 +1502,308 @@
   </sheetPr>
   <dimension ref="A1:H200"/>
   <sheetViews>
-    <sheetView view="pageBreakPreview" topLeftCell="A9" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A17" zoomScale="85" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26:E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="28.6666666666667" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="28.6640625" defaultRowHeight="13.8"/>
   <cols>
-    <col width="17.6666666666667" customWidth="1" style="100" min="1" max="1"/>
-    <col width="33.1047619047619" customWidth="1" style="100" min="2" max="2"/>
-    <col width="42.552380952381" customWidth="1" style="100" min="3" max="3"/>
-    <col width="34.552380952381" customWidth="1" style="100" min="4" max="4"/>
-    <col width="47.552380952381" customWidth="1" style="100" min="5" max="5"/>
-    <col width="28.6666666666667" customWidth="1" style="100" min="6" max="16384"/>
+    <col width="17.6640625" customWidth="1" style="114" min="1" max="1"/>
+    <col width="33.109375" customWidth="1" style="114" min="2" max="2"/>
+    <col width="42.5546875" customWidth="1" style="114" min="3" max="3"/>
+    <col width="34.5546875" customWidth="1" style="114" min="4" max="4"/>
+    <col width="47.5546875" customWidth="1" style="114" min="5" max="5"/>
+    <col width="28.6640625" customWidth="1" style="114" min="6" max="6"/>
+    <col width="28.6640625" customWidth="1" style="114" min="7" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" ht="45.9" customHeight="1">
-      <c r="A1" s="101" t="inlineStr">
+    <row r="1" ht="45.9" customHeight="1" s="123">
+      <c r="A1" s="113" t="inlineStr">
         <is>
           <t>SALES CONTRACT</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="30" customFormat="1" customHeight="1" s="98">
-      <c r="A2" s="102" t="n"/>
-      <c r="B2" s="102" t="n"/>
-      <c r="C2" s="102" t="n"/>
-      <c r="D2" s="102" t="n"/>
-      <c r="E2" s="102" t="n"/>
-    </row>
-    <row r="3" ht="27" customFormat="1" customHeight="1" s="98">
-      <c r="B3" s="103" t="n"/>
-      <c r="C3" s="103" t="n"/>
-      <c r="D3" s="104" t="inlineStr">
+    <row r="2" ht="30" customFormat="1" customHeight="1" s="88">
+      <c r="A2" s="91" t="n"/>
+      <c r="B2" s="91" t="n"/>
+      <c r="C2" s="91" t="n"/>
+      <c r="D2" s="91" t="n"/>
+      <c r="E2" s="91" t="n"/>
+    </row>
+    <row r="3" ht="27" customFormat="1" customHeight="1" s="88">
+      <c r="B3" s="92" t="n"/>
+      <c r="C3" s="92" t="n"/>
+      <c r="D3" s="93" t="inlineStr">
         <is>
           <t>DATE:</t>
         </is>
       </c>
-      <c r="E3" s="128">
+      <c r="E3" s="142">
         <f>Invoice!G9</f>
         <v/>
       </c>
     </row>
-    <row r="4" ht="30" customFormat="1" customHeight="1" s="98">
-      <c r="A4" s="103" t="n"/>
-      <c r="B4" s="103" t="n"/>
-      <c r="C4" s="103" t="n"/>
-      <c r="D4" s="104" t="inlineStr">
+    <row r="4" ht="30" customFormat="1" customHeight="1" s="88">
+      <c r="A4" s="92" t="n"/>
+      <c r="B4" s="92" t="n"/>
+      <c r="C4" s="92" t="n"/>
+      <c r="D4" s="93" t="inlineStr">
         <is>
           <t>CONTRACT NO.:</t>
         </is>
       </c>
-      <c r="E4" s="106">
+      <c r="E4" s="95">
         <f>Invoice!G8</f>
         <v/>
       </c>
     </row>
-    <row r="5" ht="32.1" customFormat="1" customHeight="1" s="99">
-      <c r="A5" s="107" t="inlineStr">
+    <row r="5" ht="32.1" customFormat="1" customHeight="1" s="116">
+      <c r="A5" s="96" t="inlineStr">
         <is>
           <t xml:space="preserve">The Seller:   </t>
         </is>
       </c>
-      <c r="B5" s="99" t="inlineStr">
+      <c r="B5" s="116" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
     </row>
-    <row r="6" ht="32.1" customFormat="1" customHeight="1" s="99">
-      <c r="B6" s="99" t="inlineStr">
+    <row r="6" ht="32.1" customFormat="1" customHeight="1" s="116">
+      <c r="B6" s="116" t="inlineStr">
         <is>
           <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District,</t>
         </is>
       </c>
     </row>
-    <row r="7" ht="32.1" customFormat="1" customHeight="1" s="99">
-      <c r="B7" s="99" t="inlineStr">
+    <row r="7" ht="32.1" customFormat="1" customHeight="1" s="116">
+      <c r="B7" s="116" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="32.1" customFormat="1" customHeight="1" s="99">
-      <c r="A8" s="107" t="inlineStr">
+    <row r="8" ht="32.1" customFormat="1" customHeight="1" s="116">
+      <c r="A8" s="96" t="inlineStr">
         <is>
           <t>TEL:</t>
         </is>
       </c>
-      <c r="B8" s="108" t="inlineStr">
+      <c r="B8" s="97" t="inlineStr">
         <is>
           <t>+855   975910636</t>
         </is>
       </c>
-      <c r="C8" s="109" t="n"/>
-      <c r="D8" s="109" t="n"/>
-      <c r="E8" s="109" t="n"/>
-    </row>
-    <row r="9" ht="32.1" customFormat="1" customHeight="1" s="99">
-      <c r="A9" s="107" t="inlineStr">
+      <c r="C8" s="98" t="n"/>
+      <c r="D8" s="98" t="n"/>
+      <c r="E8" s="98" t="n"/>
+    </row>
+    <row r="9" ht="32.1" customFormat="1" customHeight="1" s="116">
+      <c r="A9" s="96" t="inlineStr">
         <is>
           <t xml:space="preserve">The Buyer:  </t>
         </is>
       </c>
-      <c r="B9" s="99" t="inlineStr">
+      <c r="B9" s="116" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="45" customFormat="1" customHeight="1" s="99">
-      <c r="A10" s="107" t="n"/>
-      <c r="B10" s="110" t="inlineStr">
+    <row r="10" ht="45" customFormat="1" customHeight="1" s="116">
+      <c r="A10" s="96" t="n"/>
+      <c r="B10" s="115" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="32.1" customFormat="1" customHeight="1" s="99">
-      <c r="A11" s="107" t="n"/>
-      <c r="B11" s="110" t="inlineStr">
+    <row r="11" ht="32.1" customFormat="1" customHeight="1" s="116">
+      <c r="A11" s="96" t="n"/>
+      <c r="B11" s="115" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD, DONG NAI PROVINCE, VIETNAM</t>
         </is>
       </c>
     </row>
-    <row r="12" ht="30" customFormat="1" customHeight="1" s="99">
-      <c r="A12" s="99" t="inlineStr">
+    <row r="12" ht="30" customFormat="1" customHeight="1" s="116">
+      <c r="A12" s="116" t="inlineStr">
         <is>
           <t>Contact Person : Contact Person : Mr. Thuy   Tel: 0379367084</t>
         </is>
       </c>
-      <c r="E12" s="107" t="n"/>
-    </row>
-    <row r="13" ht="60.9" customFormat="1" customHeight="1" s="99">
-      <c r="A13" s="111" t="inlineStr">
+      <c r="E12" s="96" t="n"/>
+    </row>
+    <row r="13" ht="60.9" customFormat="1" customHeight="1" s="116">
+      <c r="A13" s="117" t="inlineStr">
         <is>
           <t>EMAll:jyangbin4720@dingtalk.com jialy@kukahome.com dailin@kukahome.com huanggf@kukahome.com zhangzp@kukahome.com</t>
         </is>
       </c>
     </row>
-    <row r="14" ht="54.9" customFormat="1" customHeight="1" s="99">
-      <c r="A14" s="112" t="inlineStr">
+    <row r="14" ht="54.9" customFormat="1" customHeight="1" s="116">
+      <c r="A14" s="118" t="inlineStr">
         <is>
           <t>The undersigned Sellers 、Buyers and Beneficiary have agreed to close the  following transactions according to the terms and conditions Stipulated below:</t>
         </is>
       </c>
     </row>
-    <row r="15" ht="36" customHeight="1"/>
-    <row r="16" ht="30" customHeight="1"/>
-    <row r="17" ht="30" customFormat="1" customHeight="1" s="99">
-      <c r="A17" s="129" t="n"/>
-      <c r="C17" s="130" t="n"/>
-      <c r="D17" s="130" t="n"/>
-      <c r="E17" s="130" t="n"/>
-    </row>
-    <row r="18" ht="30" customFormat="1" customHeight="1" s="99">
-      <c r="A18" s="120" t="inlineStr">
+    <row r="15" ht="36" customHeight="1" s="123"/>
+    <row r="16" ht="30" customHeight="1" s="123"/>
+    <row r="17" ht="30" customFormat="1" customHeight="1" s="116">
+      <c r="A17" s="143" t="n"/>
+      <c r="C17" s="144" t="n"/>
+      <c r="D17" s="144" t="n"/>
+      <c r="E17" s="144" t="n"/>
+    </row>
+    <row r="18" ht="30" customFormat="1" customHeight="1" s="116">
+      <c r="A18" s="106" t="inlineStr">
         <is>
           <t>FCA:</t>
         </is>
       </c>
-      <c r="B18" s="121" t="inlineStr">
+      <c r="B18" s="107" t="inlineStr">
         <is>
           <t>BAVET, SVAY RIENG</t>
         </is>
       </c>
-      <c r="C18" s="107" t="n"/>
-      <c r="D18" s="107" t="n"/>
-      <c r="E18" s="107" t="n"/>
-    </row>
-    <row r="19" ht="30" customFormat="1" customHeight="1" s="99">
-      <c r="A19" s="107" t="inlineStr">
+      <c r="C18" s="96" t="n"/>
+      <c r="D18" s="96" t="n"/>
+      <c r="E18" s="96" t="n"/>
+    </row>
+    <row r="19" ht="30" customFormat="1" customHeight="1" s="116">
+      <c r="A19" s="96" t="inlineStr">
         <is>
           <t>Term of Payment: 100% TT after shipment</t>
         </is>
       </c>
-      <c r="B19" s="107" t="n"/>
-      <c r="C19" s="107" t="n"/>
-      <c r="D19" s="107" t="n"/>
-      <c r="E19" s="107" t="n"/>
-    </row>
-    <row r="20" ht="36" customHeight="1">
-      <c r="A20" s="107" t="inlineStr">
+      <c r="B19" s="96" t="n"/>
+      <c r="C19" s="96" t="n"/>
+      <c r="D19" s="96" t="n"/>
+      <c r="E19" s="96" t="n"/>
+    </row>
+    <row r="20" ht="36" customHeight="1" s="123">
+      <c r="A20" s="96" t="inlineStr">
         <is>
           <t>Transaction method: FCA(USD)</t>
         </is>
       </c>
-      <c r="B20" s="107" t="n"/>
-      <c r="C20" s="107" t="n"/>
-      <c r="D20" s="107" t="n"/>
-      <c r="E20" s="107" t="n"/>
-    </row>
-    <row r="21" ht="20.25" customHeight="1">
-      <c r="A21" s="107" t="inlineStr">
+      <c r="B20" s="96" t="n"/>
+      <c r="C20" s="96" t="n"/>
+      <c r="D20" s="96" t="n"/>
+      <c r="E20" s="96" t="n"/>
+    </row>
+    <row r="21" ht="20.4" customHeight="1" s="123">
+      <c r="A21" s="96" t="inlineStr">
         <is>
           <t xml:space="preserve">Beneficiary bank information: </t>
         </is>
       </c>
-      <c r="B21" s="107" t="n"/>
-      <c r="C21" s="107" t="inlineStr">
+      <c r="B21" s="96" t="n"/>
+      <c r="C21" s="96" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
-      <c r="D21" s="107" t="n"/>
-      <c r="E21" s="107" t="n"/>
-    </row>
-    <row r="22" ht="45.9" customHeight="1">
-      <c r="A22" s="107" t="inlineStr">
+      <c r="D21" s="96" t="n"/>
+      <c r="E21" s="96" t="n"/>
+    </row>
+    <row r="22" ht="45.9" customHeight="1" s="123">
+      <c r="A22" s="96" t="inlineStr">
         <is>
           <t xml:space="preserve">Beneficiary Bank' s Name: </t>
         </is>
       </c>
-      <c r="B22" s="107" t="n"/>
-      <c r="C22" s="112" t="inlineStr">
+      <c r="B22" s="96" t="n"/>
+      <c r="C22" s="118" t="inlineStr">
         <is>
           <t>BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
  /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
     </row>
-    <row r="23" ht="41.1" customHeight="1">
-      <c r="A23" s="107" t="inlineStr">
+    <row r="23" ht="41.1" customHeight="1" s="123">
+      <c r="A23" s="96" t="inlineStr">
         <is>
           <t xml:space="preserve">Bank Address:  </t>
         </is>
       </c>
-      <c r="B23" s="107" t="n"/>
-      <c r="C23" s="112" t="inlineStr">
+      <c r="B23" s="96" t="n"/>
+      <c r="C23" s="118" t="inlineStr">
         <is>
           <t>1st AND 2nd FLOOR,CANADIA TOWER,No.315 ANDDUONG ST.
 PHNOM PEMH,CAMBODIA.</t>
         </is>
       </c>
     </row>
-    <row r="24" ht="29.1" customHeight="1">
-      <c r="A24" s="107" t="inlineStr">
+    <row r="24" ht="29.1" customHeight="1" s="123">
+      <c r="A24" s="96" t="inlineStr">
         <is>
           <t>Bank account :</t>
         </is>
       </c>
-      <c r="B24" s="107" t="n"/>
-      <c r="C24" s="122" t="inlineStr">
+      <c r="B24" s="96" t="n"/>
+      <c r="C24" s="121" t="inlineStr">
         <is>
           <t>100001100764430</t>
         </is>
       </c>
     </row>
-    <row r="25" ht="19.5" customHeight="1">
-      <c r="A25" s="107" t="inlineStr">
+    <row r="25" ht="19.2" customHeight="1" s="123">
+      <c r="A25" s="96" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：</t>
         </is>
       </c>
-      <c r="B25" s="107" t="n"/>
-      <c r="C25" s="107" t="inlineStr">
+      <c r="B25" s="96" t="n"/>
+      <c r="C25" s="96" t="inlineStr">
         <is>
           <t>BKCHKHPPXXX</t>
         </is>
       </c>
-      <c r="D25" s="107" t="n"/>
-      <c r="E25" s="107" t="n"/>
-    </row>
-    <row r="26" ht="45.9" customHeight="1">
-      <c r="A26" s="107" t="n"/>
-      <c r="B26" s="107" t="n"/>
-      <c r="C26" s="107" t="n"/>
-      <c r="D26" s="107" t="n"/>
-      <c r="E26" s="107" t="n"/>
-      <c r="F26" s="107" t="n"/>
-    </row>
-    <row r="27" ht="41.1" customHeight="1">
-      <c r="A27" s="123" t="inlineStr">
+      <c r="D25" s="96" t="n"/>
+      <c r="E25" s="96" t="n"/>
+    </row>
+    <row r="26" ht="45.9" customHeight="1" s="123">
+      <c r="A26" s="96" t="n"/>
+      <c r="B26" s="96" t="n"/>
+      <c r="C26" s="96" t="n"/>
+      <c r="D26" s="96" t="n"/>
+      <c r="E26" s="96" t="n"/>
+      <c r="F26" s="96" t="n"/>
+    </row>
+    <row r="27" ht="41.1" customHeight="1" s="123">
+      <c r="A27" s="108" t="inlineStr">
         <is>
           <t>The Buyer:</t>
         </is>
       </c>
-      <c r="D27" s="124" t="inlineStr">
+      <c r="D27" s="109" t="inlineStr">
         <is>
           <t>The Seller:</t>
         </is>
       </c>
     </row>
-    <row r="28" ht="29.1" customHeight="1">
-      <c r="A28" s="125" t="inlineStr">
+    <row r="28" ht="29.1" customHeight="1" s="123">
+      <c r="A28" s="110" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
       </c>
-      <c r="B28" s="126" t="n"/>
-      <c r="C28" s="127" t="n"/>
-      <c r="D28" s="125" t="inlineStr">
+      <c r="B28" s="111" t="n"/>
+      <c r="C28" s="112" t="n"/>
+      <c r="D28" s="110" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO.,LTD.</t>
         </is>
       </c>
-      <c r="E28" s="125" t="n"/>
-    </row>
-    <row r="29" ht="19.5" customHeight="1"/>
-    <row r="30" ht="19.5" customHeight="1"/>
-    <row r="31" ht="20.25" customHeight="1"/>
-    <row r="32" ht="20.25" customHeight="1"/>
+      <c r="E28" s="110" t="n"/>
+    </row>
+    <row r="29" ht="19.2" customHeight="1" s="123"/>
+    <row r="30" ht="19.2" customHeight="1" s="123"/>
+    <row r="31" ht="21" customHeight="1" s="123"/>
+    <row r="32" ht="21" customHeight="1" s="123"/>
     <row r="33"/>
     <row r="34"/>
     <row r="35"/>
@@ -2533,7 +1960,7 @@
     <row r="186"/>
     <row r="187"/>
     <row r="188"/>
-    <row r="189" ht="27.9" customHeight="1"/>
+    <row r="189" ht="27.9" customHeight="1" s="123"/>
     <row r="190"/>
     <row r="191"/>
     <row r="192"/>
@@ -2544,7 +1971,7 @@
     <row r="197"/>
     <row r="198"/>
     <row r="199"/>
-    <row r="200" ht="27.9" customHeight="1"/>
+    <row r="200" ht="27.9" customHeight="1" s="123"/>
   </sheetData>
   <mergeCells count="13">
     <mergeCell ref="C28:E28"/>
@@ -2553,8 +1980,8 @@
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="A1:E1"/>
+    <mergeCell ref="C26:E26"/>
     <mergeCell ref="B11:E11"/>
-    <mergeCell ref="C26:E26"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
     <mergeCell ref="A189:B189"/>
@@ -2578,430 +2005,430 @@
       <selection activeCell="G22" sqref="G22:G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="7.1047619047619" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="7.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="24.3333333333333" customWidth="1" min="1" max="1"/>
-    <col width="28.1047619047619" customWidth="1" min="2" max="2"/>
-    <col width="21.6666666666667" customWidth="1" min="3" max="3"/>
-    <col width="18.3333333333333" customWidth="1" min="4" max="4"/>
-    <col width="15.6666666666667" customWidth="1" min="5" max="5"/>
-    <col width="16.4380952380952" customWidth="1" min="6" max="6"/>
-    <col width="24.8857142857143" customWidth="1" style="3" min="7" max="7"/>
-    <col width="25.1047619047619" customWidth="1" min="8" max="8"/>
-    <col width="15.552380952381" customWidth="1" min="9" max="9"/>
-    <col width="10.3333333333333" customWidth="1" min="10" max="10"/>
-    <col width="12.4380952380952" customWidth="1" min="12" max="12"/>
+    <col width="24.33203125" customWidth="1" style="123" min="1" max="1"/>
+    <col width="28.109375" customWidth="1" style="123" min="2" max="2"/>
+    <col width="21.6640625" customWidth="1" style="123" min="3" max="3"/>
+    <col width="18.33203125" customWidth="1" style="123" min="4" max="4"/>
+    <col width="15.6640625" customWidth="1" style="123" min="5" max="5"/>
+    <col width="16.44140625" customWidth="1" style="123" min="6" max="6"/>
+    <col width="24.88671875" customWidth="1" style="124" min="7" max="7"/>
+    <col width="25.109375" customWidth="1" style="123" min="8" max="8"/>
+    <col width="15.5546875" customWidth="1" style="123" min="9" max="9"/>
+    <col width="10.33203125" customWidth="1" style="123" min="10" max="10"/>
+    <col width="12.44140625" customWidth="1" style="123" min="12" max="12"/>
   </cols>
   <sheetData>
-    <row r="1" ht="38.25" customHeight="1">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" ht="38.25" customHeight="1" s="123">
+      <c r="A1" s="122" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="24" customHeight="1">
-      <c r="A2" s="6" t="inlineStr">
+    <row r="2" ht="24" customHeight="1" s="123">
+      <c r="A2" s="125" t="inlineStr">
         <is>
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
         </is>
       </c>
     </row>
-    <row r="3" ht="17.25" customHeight="1">
-      <c r="A3" s="7" t="inlineStr">
+    <row r="3" ht="17.25" customHeight="1" s="123">
+      <c r="A3" s="126" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="17.25" customHeight="1">
-      <c r="A4" s="6" t="inlineStr">
+    <row r="4" ht="17.25" customHeight="1" s="123">
+      <c r="A4" s="125" t="inlineStr">
         <is>
           <t>VAT:L001-901903209</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="8" t="inlineStr">
+    <row r="5" ht="25.5" customHeight="1" s="123">
+      <c r="A5" s="127" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="B5" s="9" t="n"/>
-      <c r="C5" s="9" t="n"/>
-      <c r="D5" s="9" t="n"/>
-      <c r="E5" s="9" t="n"/>
-      <c r="F5" s="9" t="n"/>
-      <c r="G5" s="9" t="n"/>
-    </row>
-    <row r="6" ht="83.25" customHeight="1">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="B5" s="128" t="n"/>
+      <c r="C5" s="128" t="n"/>
+      <c r="D5" s="128" t="n"/>
+      <c r="E5" s="128" t="n"/>
+      <c r="F5" s="128" t="n"/>
+      <c r="G5" s="128" t="n"/>
+    </row>
+    <row r="6" ht="83.25" customHeight="1" s="123">
+      <c r="A6" s="129" t="inlineStr">
         <is>
           <t>INVOICE</t>
         </is>
       </c>
-      <c r="B6" s="11" t="n"/>
-      <c r="C6" s="11" t="n"/>
-      <c r="D6" s="11" t="n"/>
-      <c r="E6" s="11" t="n"/>
-      <c r="F6" s="11" t="n"/>
-      <c r="G6" s="11" t="n"/>
-    </row>
-    <row r="7" ht="14.25" customHeight="1">
-      <c r="A7" s="12" t="n"/>
-      <c r="B7" s="12" t="n"/>
-      <c r="C7" s="12" t="n"/>
-      <c r="D7" s="12" t="n"/>
-      <c r="E7" s="12" t="n"/>
-      <c r="F7" s="14" t="inlineStr">
+      <c r="B6" s="130" t="n"/>
+      <c r="C6" s="130" t="n"/>
+      <c r="D6" s="130" t="n"/>
+      <c r="E6" s="130" t="n"/>
+      <c r="F6" s="130" t="n"/>
+      <c r="G6" s="130" t="n"/>
+    </row>
+    <row r="7" ht="14.25" customHeight="1" s="123">
+      <c r="A7" s="6" t="n"/>
+      <c r="B7" s="6" t="n"/>
+      <c r="C7" s="6" t="n"/>
+      <c r="D7" s="6" t="n"/>
+      <c r="E7" s="6" t="n"/>
+      <c r="F7" s="8" t="inlineStr">
         <is>
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="G7" s="74">
+      <c r="G7" s="64">
         <f>'Packing list'!I7</f>
         <v/>
       </c>
     </row>
-    <row r="8" ht="30" customHeight="1">
-      <c r="A8" s="15" t="inlineStr">
+    <row r="8" ht="30" customHeight="1" s="123">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="75" t="inlineStr">
+      <c r="B8" s="65" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="E8" s="75" t="n"/>
-      <c r="F8" s="17" t="inlineStr">
+      <c r="E8" s="65" t="n"/>
+      <c r="F8" s="11" t="inlineStr">
         <is>
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="G8" s="76">
+      <c r="G8" s="66">
         <f>'Packing list'!I8</f>
         <v/>
       </c>
     </row>
-    <row r="9" ht="21" customHeight="1">
-      <c r="A9" s="12" t="n"/>
-      <c r="B9" s="12" t="inlineStr">
+    <row r="9" ht="21" customHeight="1" s="123">
+      <c r="A9" s="6" t="n"/>
+      <c r="B9" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve">XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, </t>
         </is>
       </c>
-      <c r="E9" s="12" t="n"/>
-      <c r="F9" s="17" t="inlineStr">
+      <c r="E9" s="6" t="n"/>
+      <c r="F9" s="11" t="inlineStr">
         <is>
           <t>Date:</t>
         </is>
       </c>
-      <c r="G9" s="131">
+      <c r="G9" s="145">
         <f>'Packing list'!I9</f>
         <v/>
       </c>
     </row>
-    <row r="10" ht="22.5" customHeight="1">
-      <c r="A10" s="12" t="n"/>
-      <c r="B10" s="12" t="inlineStr">
+    <row r="10" ht="22.5" customHeight="1" s="123">
+      <c r="A10" s="6" t="n"/>
+      <c r="B10" s="6" t="inlineStr">
         <is>
           <t xml:space="preserve">Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia </t>
         </is>
       </c>
-      <c r="E10" s="12" t="n"/>
-      <c r="F10" s="18" t="inlineStr">
+      <c r="E10" s="6" t="n"/>
+      <c r="F10" s="12" t="inlineStr">
         <is>
           <t>FCA :</t>
         </is>
       </c>
-      <c r="G10" s="77" t="inlineStr">
+      <c r="G10" s="67" t="inlineStr">
         <is>
           <t>BAVET, SVAYRIENG</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="12" t="n"/>
-      <c r="B11" s="12" t="inlineStr">
+    <row r="11" ht="20.25" customHeight="1" s="123">
+      <c r="A11" s="6" t="n"/>
+      <c r="B11" s="6" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="E11" s="12" t="n"/>
-      <c r="F11" s="12" t="n"/>
-      <c r="G11" s="6" t="n"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="12" t="n"/>
-      <c r="B12" s="12" t="n"/>
-      <c r="C12" s="12" t="n"/>
-      <c r="D12" s="12" t="n"/>
-      <c r="E12" s="12" t="n"/>
-      <c r="F12" s="12" t="n"/>
-      <c r="G12" s="6" t="n"/>
-    </row>
-    <row r="13" ht="25.5" customHeight="1">
-      <c r="A13" s="19" t="inlineStr">
+      <c r="E11" s="6" t="n"/>
+      <c r="F11" s="6" t="n"/>
+      <c r="G11" s="125" t="n"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" s="123">
+      <c r="A12" s="6" t="n"/>
+      <c r="B12" s="6" t="n"/>
+      <c r="C12" s="6" t="n"/>
+      <c r="D12" s="6" t="n"/>
+      <c r="E12" s="6" t="n"/>
+      <c r="F12" s="6" t="n"/>
+      <c r="G12" s="125" t="n"/>
+    </row>
+    <row r="13" ht="25.5" customHeight="1" s="123">
+      <c r="A13" s="13" t="inlineStr">
         <is>
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="78" t="inlineStr">
+      <c r="B13" s="68" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
       </c>
-      <c r="E13" s="79" t="n"/>
-      <c r="F13" s="79" t="n"/>
-      <c r="G13" s="27" t="n"/>
-    </row>
-    <row r="14" ht="25.5" customHeight="1">
-      <c r="A14" s="12" t="n"/>
-      <c r="B14" s="80" t="inlineStr">
+      <c r="E13" s="69" t="n"/>
+      <c r="F13" s="69" t="n"/>
+      <c r="G13" s="21" t="n"/>
+    </row>
+    <row r="14" ht="25.5" customHeight="1" s="123">
+      <c r="A14" s="6" t="n"/>
+      <c r="B14" s="70" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
-      <c r="C14" s="23" t="n"/>
-      <c r="D14" s="23" t="n"/>
-      <c r="E14" s="23" t="n"/>
-      <c r="F14" s="23" t="n"/>
-    </row>
-    <row r="15" ht="25.5" customHeight="1">
-      <c r="A15" s="12" t="n"/>
-      <c r="B15" s="28" t="inlineStr">
+      <c r="C14" s="17" t="n"/>
+      <c r="D14" s="17" t="n"/>
+      <c r="E14" s="17" t="n"/>
+      <c r="F14" s="17" t="n"/>
+    </row>
+    <row r="15" ht="25.5" customHeight="1" s="123">
+      <c r="A15" s="6" t="n"/>
+      <c r="B15" s="22" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
         </is>
       </c>
-      <c r="C15" s="26" t="n"/>
-      <c r="D15" s="26" t="n"/>
-      <c r="E15" s="26" t="n"/>
-      <c r="F15" s="27" t="n"/>
-    </row>
-    <row r="16" ht="25.5" customHeight="1">
-      <c r="A16" s="12" t="n"/>
-      <c r="B16" s="52" t="inlineStr">
+      <c r="C15" s="20" t="n"/>
+      <c r="D15" s="20" t="n"/>
+      <c r="E15" s="20" t="n"/>
+      <c r="F15" s="21" t="n"/>
+    </row>
+    <row r="16" ht="25.5" customHeight="1" s="123">
+      <c r="A16" s="6" t="n"/>
+      <c r="B16" s="42" t="inlineStr">
         <is>
           <t>Contact Person : Mr. Thuy   TEl: 0379367084</t>
         </is>
       </c>
-      <c r="C16" s="26" t="n"/>
-      <c r="D16" s="26" t="n"/>
-      <c r="E16" s="26" t="n"/>
-      <c r="F16" s="26" t="n"/>
-    </row>
-    <row r="17" ht="25.5" customHeight="1">
-      <c r="A17" s="12" t="n"/>
-      <c r="B17" s="52" t="inlineStr">
+      <c r="C16" s="20" t="n"/>
+      <c r="D16" s="20" t="n"/>
+      <c r="E16" s="20" t="n"/>
+      <c r="F16" s="20" t="n"/>
+    </row>
+    <row r="17" ht="25.5" customHeight="1" s="123">
+      <c r="A17" s="6" t="n"/>
+      <c r="B17" s="42" t="inlineStr">
         <is>
           <t xml:space="preserve">EMAlL:jyangbin4720@dingtalk.com jialy@kukahome.com </t>
         </is>
       </c>
-      <c r="C17" s="26" t="n"/>
-      <c r="D17" s="26" t="n"/>
-      <c r="E17" s="26" t="n"/>
-      <c r="F17" s="27" t="n"/>
-    </row>
-    <row r="18" ht="25.5" customHeight="1">
-      <c r="A18" s="12" t="n"/>
-      <c r="B18" s="52" t="inlineStr">
+      <c r="C17" s="20" t="n"/>
+      <c r="D17" s="20" t="n"/>
+      <c r="E17" s="20" t="n"/>
+      <c r="F17" s="21" t="n"/>
+    </row>
+    <row r="18" ht="25.5" customHeight="1" s="123">
+      <c r="A18" s="6" t="n"/>
+      <c r="B18" s="42" t="inlineStr">
         <is>
           <t>dailin@kukahome.com huanggf@kukahome.com zhangzp@kukahome.com</t>
         </is>
       </c>
-      <c r="C18" s="12" t="n"/>
-      <c r="D18" s="12" t="n"/>
-      <c r="E18" s="12" t="n"/>
-      <c r="F18" s="6" t="n"/>
-    </row>
-    <row r="19" ht="27.75" customHeight="1">
-      <c r="A19" s="29" t="inlineStr">
+      <c r="C18" s="6" t="n"/>
+      <c r="D18" s="6" t="n"/>
+      <c r="E18" s="6" t="n"/>
+      <c r="F18" s="125" t="n"/>
+    </row>
+    <row r="19" ht="27.75" customHeight="1" s="123">
+      <c r="A19" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B19" s="12" t="inlineStr">
+      <c r="B19" s="6" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
         </is>
       </c>
-      <c r="F19" s="3" t="n"/>
-    </row>
-    <row r="20" ht="27.75" customHeight="1">
-      <c r="A20" s="30" t="n"/>
-      <c r="B20" s="30" t="n"/>
-    </row>
-    <row r="21" ht="34.95" customHeight="1"/>
-    <row r="22" ht="34.95" customHeight="1"/>
-    <row r="23" ht="34.95" customHeight="1">
-      <c r="A23" s="61" t="n"/>
-      <c r="B23" s="61" t="n"/>
-      <c r="C23" s="83" t="n"/>
-      <c r="D23" s="83" t="n"/>
-      <c r="E23" s="83" t="n"/>
-      <c r="F23" s="83" t="n"/>
-      <c r="G23" s="27" t="n"/>
-      <c r="L23" s="95" t="n"/>
-      <c r="M23" s="96" t="n"/>
-      <c r="N23" s="97" t="n"/>
-      <c r="O23" s="97" t="n"/>
-    </row>
-    <row r="24" ht="42" customHeight="1">
-      <c r="A24" s="46" t="inlineStr">
+      <c r="F19" s="124" t="n"/>
+    </row>
+    <row r="20" ht="27.75" customHeight="1" s="123">
+      <c r="A20" s="24" t="n"/>
+      <c r="B20" s="24" t="n"/>
+    </row>
+    <row r="21" ht="34.95" customHeight="1" s="123"/>
+    <row r="22" ht="34.95" customHeight="1" s="123"/>
+    <row r="23" ht="34.95" customHeight="1" s="123">
+      <c r="A23" s="51" t="n"/>
+      <c r="B23" s="51" t="n"/>
+      <c r="C23" s="73" t="n"/>
+      <c r="D23" s="73" t="n"/>
+      <c r="E23" s="73" t="n"/>
+      <c r="F23" s="73" t="n"/>
+      <c r="G23" s="21" t="n"/>
+      <c r="L23" s="85" t="n"/>
+      <c r="M23" s="86" t="n"/>
+      <c r="N23" s="87" t="n"/>
+      <c r="O23" s="87" t="n"/>
+    </row>
+    <row r="24" ht="42" customHeight="1" s="123">
+      <c r="A24" s="131" t="inlineStr">
         <is>
           <t>Country of Original Cambodia</t>
         </is>
       </c>
-      <c r="D24" s="46" t="n"/>
-      <c r="E24" s="12" t="n"/>
-      <c r="F24" s="84" t="n"/>
-      <c r="G24" s="6" t="n"/>
-      <c r="L24" s="95" t="n"/>
-      <c r="M24" s="96" t="n"/>
-      <c r="N24" s="97" t="n"/>
-      <c r="O24" s="97" t="n"/>
-    </row>
-    <row r="25" ht="61.5" customHeight="1">
-      <c r="A25" s="48" t="inlineStr">
+      <c r="D24" s="131" t="n"/>
+      <c r="E24" s="6" t="n"/>
+      <c r="F24" s="74" t="n"/>
+      <c r="G24" s="125" t="n"/>
+      <c r="L24" s="85" t="n"/>
+      <c r="M24" s="86" t="n"/>
+      <c r="N24" s="87" t="n"/>
+      <c r="O24" s="87" t="n"/>
+    </row>
+    <row r="25" ht="61.5" customHeight="1" s="123">
+      <c r="A25" s="39" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B25" s="85" t="inlineStr">
+      <c r="B25" s="132" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="D25" s="85" t="n"/>
-      <c r="E25" s="85" t="n"/>
-      <c r="F25" s="12" t="n"/>
-      <c r="G25" s="6" t="n"/>
-      <c r="L25" s="95" t="n"/>
-      <c r="M25" s="96" t="n"/>
-      <c r="N25" s="97" t="n"/>
-      <c r="O25" s="97" t="n"/>
-    </row>
-    <row r="26" ht="42" customHeight="1">
-      <c r="A26" s="86" t="inlineStr">
+      <c r="D25" s="132" t="n"/>
+      <c r="E25" s="132" t="n"/>
+      <c r="F25" s="6" t="n"/>
+      <c r="G25" s="125" t="n"/>
+      <c r="L25" s="85" t="n"/>
+      <c r="M25" s="86" t="n"/>
+      <c r="N25" s="87" t="n"/>
+      <c r="O25" s="87" t="n"/>
+    </row>
+    <row r="26" ht="42" customHeight="1" s="123">
+      <c r="A26" s="133" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED PHNOM PENH BRANCH
                                                   /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="D26" s="86" t="n"/>
-      <c r="E26" s="86" t="n"/>
-      <c r="F26" s="86" t="n"/>
-      <c r="G26" s="6" t="n"/>
-      <c r="L26" s="95" t="n"/>
-      <c r="M26" s="96" t="n"/>
-      <c r="N26" s="97" t="n"/>
-      <c r="O26" s="97" t="n"/>
-    </row>
-    <row r="27" ht="24.75" customHeight="1">
-      <c r="A27" s="51" t="inlineStr">
+      <c r="D26" s="133" t="n"/>
+      <c r="E26" s="133" t="n"/>
+      <c r="F26" s="133" t="n"/>
+      <c r="G26" s="125" t="n"/>
+      <c r="L26" s="85" t="n"/>
+      <c r="M26" s="86" t="n"/>
+      <c r="N26" s="87" t="n"/>
+      <c r="O26" s="87" t="n"/>
+    </row>
+    <row r="27" ht="24.75" customHeight="1" s="123">
+      <c r="A27" s="134" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
-      <c r="L27" s="95" t="n"/>
-      <c r="M27" s="96" t="n"/>
-      <c r="N27" s="97" t="n"/>
-      <c r="O27" s="97" t="n"/>
-    </row>
-    <row r="28" ht="27" customHeight="1">
-      <c r="A28" s="51" t="inlineStr">
+      <c r="L27" s="85" t="n"/>
+      <c r="M27" s="86" t="n"/>
+      <c r="N27" s="87" t="n"/>
+      <c r="O27" s="87" t="n"/>
+    </row>
+    <row r="28" ht="27" customHeight="1" s="123">
+      <c r="A28" s="134" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
       </c>
-      <c r="L28" s="95" t="n"/>
-      <c r="M28" s="96" t="n"/>
-      <c r="N28" s="97" t="n"/>
-      <c r="O28" s="97" t="n"/>
-    </row>
-    <row r="29" ht="61.5" customHeight="1">
-      <c r="E29" s="87" t="inlineStr">
+      <c r="L28" s="85" t="n"/>
+      <c r="M28" s="86" t="n"/>
+      <c r="N28" s="87" t="n"/>
+      <c r="O28" s="87" t="n"/>
+    </row>
+    <row r="29" ht="61.5" customHeight="1" s="123">
+      <c r="E29" s="77" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="F29" s="87" t="n"/>
-      <c r="G29" s="87" t="n"/>
-      <c r="H29" s="87" t="n"/>
-      <c r="L29" s="95" t="n"/>
-      <c r="M29" s="96" t="n"/>
-      <c r="N29" s="97" t="n"/>
-      <c r="O29" s="97" t="n"/>
-    </row>
-    <row r="30" ht="42" customHeight="1">
-      <c r="D30" s="88" t="n"/>
-      <c r="E30" s="89" t="n"/>
-      <c r="F30" s="90" t="inlineStr">
+      <c r="F29" s="77" t="n"/>
+      <c r="G29" s="77" t="n"/>
+      <c r="H29" s="77" t="n"/>
+      <c r="L29" s="85" t="n"/>
+      <c r="M29" s="86" t="n"/>
+      <c r="N29" s="87" t="n"/>
+      <c r="O29" s="87" t="n"/>
+    </row>
+    <row r="30" ht="42" customHeight="1" s="123">
+      <c r="D30" s="78" t="n"/>
+      <c r="E30" s="79" t="n"/>
+      <c r="F30" s="80" t="inlineStr">
         <is>
           <t>Sign &amp; Stamp</t>
         </is>
       </c>
-      <c r="G30" s="91" t="n"/>
-      <c r="L30" s="95" t="n"/>
-      <c r="M30" s="96" t="n"/>
-      <c r="N30" s="97" t="n"/>
-      <c r="O30" s="97" t="n"/>
-    </row>
-    <row r="31" ht="24.75" customHeight="1">
-      <c r="D31" s="88" t="n"/>
-      <c r="E31" s="89" t="n"/>
-      <c r="F31" s="89" t="n"/>
-      <c r="G31" s="91" t="n"/>
-      <c r="L31" s="95" t="n"/>
-      <c r="M31" s="96" t="n"/>
-      <c r="N31" s="97" t="n"/>
-      <c r="O31" s="97" t="n"/>
-    </row>
-    <row r="32" ht="27" customHeight="1">
-      <c r="D32" s="88" t="n"/>
-      <c r="E32" s="89" t="n"/>
-      <c r="F32" s="89" t="n"/>
-      <c r="G32" s="91" t="n"/>
-      <c r="L32" s="95" t="n"/>
-      <c r="M32" s="96" t="n"/>
-      <c r="N32" s="97" t="n"/>
-      <c r="O32" s="97" t="n"/>
-    </row>
-    <row r="33" ht="21" customHeight="1">
-      <c r="D33" s="88" t="n"/>
-      <c r="E33" s="89" t="n"/>
-      <c r="F33" s="92" t="inlineStr">
+      <c r="G30" s="81" t="n"/>
+      <c r="L30" s="85" t="n"/>
+      <c r="M30" s="86" t="n"/>
+      <c r="N30" s="87" t="n"/>
+      <c r="O30" s="87" t="n"/>
+    </row>
+    <row r="31" ht="24.75" customHeight="1" s="123">
+      <c r="D31" s="78" t="n"/>
+      <c r="E31" s="79" t="n"/>
+      <c r="F31" s="79" t="n"/>
+      <c r="G31" s="81" t="n"/>
+      <c r="L31" s="85" t="n"/>
+      <c r="M31" s="86" t="n"/>
+      <c r="N31" s="87" t="n"/>
+      <c r="O31" s="87" t="n"/>
+    </row>
+    <row r="32" ht="27" customHeight="1" s="123">
+      <c r="D32" s="78" t="n"/>
+      <c r="E32" s="79" t="n"/>
+      <c r="F32" s="79" t="n"/>
+      <c r="G32" s="81" t="n"/>
+      <c r="L32" s="85" t="n"/>
+      <c r="M32" s="86" t="n"/>
+      <c r="N32" s="87" t="n"/>
+      <c r="O32" s="87" t="n"/>
+    </row>
+    <row r="33" ht="21" customHeight="1" s="123">
+      <c r="D33" s="78" t="n"/>
+      <c r="E33" s="79" t="n"/>
+      <c r="F33" s="82" t="inlineStr">
         <is>
           <t>ZENG XUELI</t>
         </is>
       </c>
-      <c r="G33" s="92" t="n"/>
-      <c r="L33" s="95" t="n"/>
-      <c r="M33" s="96" t="n"/>
-      <c r="N33" s="97" t="n"/>
-      <c r="O33" s="97" t="n"/>
-    </row>
-    <row r="34" ht="25.5" customHeight="1">
-      <c r="D34" s="93" t="n"/>
-      <c r="E34" s="93" t="n"/>
-      <c r="F34" s="93" t="n"/>
-      <c r="G34" s="94" t="n"/>
-    </row>
-    <row r="35" ht="21" customHeight="1">
-      <c r="D35" s="93" t="n"/>
-      <c r="E35" s="93" t="n"/>
-      <c r="F35" s="93" t="n"/>
-      <c r="G35" s="94" t="n"/>
-    </row>
-    <row r="36" ht="21" customHeight="1"/>
-    <row r="37" ht="21" customHeight="1"/>
-    <row r="38" ht="21" customHeight="1"/>
-    <row r="39" ht="21" customHeight="1"/>
-    <row r="40" ht="17.25" customHeight="1"/>
+      <c r="G33" s="82" t="n"/>
+      <c r="L33" s="85" t="n"/>
+      <c r="M33" s="86" t="n"/>
+      <c r="N33" s="87" t="n"/>
+      <c r="O33" s="87" t="n"/>
+    </row>
+    <row r="34" ht="25.5" customHeight="1" s="123">
+      <c r="D34" s="83" t="n"/>
+      <c r="E34" s="83" t="n"/>
+      <c r="F34" s="83" t="n"/>
+      <c r="G34" s="84" t="n"/>
+    </row>
+    <row r="35" ht="21" customHeight="1" s="123">
+      <c r="D35" s="83" t="n"/>
+      <c r="E35" s="83" t="n"/>
+      <c r="F35" s="83" t="n"/>
+      <c r="G35" s="84" t="n"/>
+    </row>
+    <row r="36" ht="21" customHeight="1" s="123"/>
+    <row r="37" ht="21" customHeight="1" s="123"/>
+    <row r="38" ht="21" customHeight="1" s="123"/>
+    <row r="39" ht="21" customHeight="1" s="123"/>
+    <row r="40" ht="17.25" customHeight="1" s="123"/>
     <row r="41"/>
     <row r="42"/>
     <row r="43"/>
@@ -3013,7 +2440,7 @@
     <row r="49"/>
     <row r="50"/>
     <row r="51"/>
-    <row r="52"/>
+    <row r="52" ht="15" customHeight="1" s="123"/>
     <row r="53"/>
     <row r="54"/>
     <row r="55"/>
@@ -3197,398 +2624,398 @@
   </sheetPr>
   <dimension ref="A1:K200"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A8" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView view="pageBreakPreview" topLeftCell="A22" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultColWidth="7.1047619047619" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="7.109375" defaultRowHeight="14.4"/>
   <cols>
-    <col width="25.4380952380952" customWidth="1" min="1" max="1"/>
-    <col width="22.8857142857143" customWidth="1" style="2" min="2" max="2"/>
-    <col width="19.4380952380952" customWidth="1" min="3" max="3"/>
-    <col width="26.6666666666667" customWidth="1" min="4" max="4"/>
-    <col width="15" customWidth="1" style="3" min="5" max="6"/>
-    <col width="13.6666666666667" customWidth="1" style="3" min="7" max="7"/>
-    <col width="15.552380952381" customWidth="1" style="3" min="8" max="8"/>
-    <col width="23.6666666666667" customWidth="1" style="3" min="9" max="9"/>
-    <col width="12.4380952380952" customWidth="1" style="4" min="10" max="10"/>
-    <col width="12.8857142857143" customWidth="1" min="11" max="11"/>
-    <col width="12.552380952381" customWidth="1" min="12" max="12"/>
-    <col width="12.552380952381" customWidth="1" min="14" max="14"/>
-    <col width="12.552380952381" customWidth="1" min="16" max="16"/>
+    <col width="25.44140625" customWidth="1" style="123" min="1" max="1"/>
+    <col width="22.88671875" customWidth="1" style="137" min="2" max="2"/>
+    <col width="19.44140625" customWidth="1" style="123" min="3" max="3"/>
+    <col width="26.6640625" customWidth="1" style="123" min="4" max="4"/>
+    <col width="15" customWidth="1" style="124" min="5" max="6"/>
+    <col width="13.6640625" customWidth="1" style="124" min="7" max="7"/>
+    <col width="15.5546875" customWidth="1" style="124" min="8" max="8"/>
+    <col width="23.6640625" customWidth="1" style="124" min="9" max="9"/>
+    <col width="12.44140625" customWidth="1" style="4" min="10" max="10"/>
+    <col width="12.88671875" customWidth="1" style="123" min="11" max="11"/>
+    <col width="12.5546875" customWidth="1" style="123" min="12" max="12"/>
+    <col width="12.5546875" customWidth="1" style="123" min="14" max="14"/>
+    <col width="12.5546875" customWidth="1" style="123" min="16" max="16"/>
   </cols>
   <sheetData>
-    <row r="1" ht="38.25" customHeight="1">
-      <c r="A1" s="5" t="inlineStr">
+    <row r="1" ht="38.25" customHeight="1" s="123">
+      <c r="A1" s="122" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
     </row>
-    <row r="2" ht="24" customHeight="1">
-      <c r="A2" s="6" t="inlineStr">
+    <row r="2" ht="24" customHeight="1" s="123">
+      <c r="A2" s="125" t="inlineStr">
         <is>
           <t xml:space="preserve"> XIN BAVET SEZ, Road No. 316A, Trapeang Bon and  Prey Kokir  Villages, Prey Kokir  Commune, Chantrea District, </t>
         </is>
       </c>
     </row>
-    <row r="3" ht="25.5" customHeight="1">
-      <c r="A3" s="7" t="inlineStr">
+    <row r="3" ht="25.5" customHeight="1" s="123">
+      <c r="A3" s="126" t="inlineStr">
         <is>
           <t>Svay Rieng Province, Kingdom of Cambodia.</t>
         </is>
       </c>
     </row>
-    <row r="4" ht="25.5" customHeight="1">
-      <c r="A4" s="6" t="inlineStr">
+    <row r="4" ht="25.5" customHeight="1" s="123">
+      <c r="A4" s="125" t="inlineStr">
         <is>
           <t>VAT:L001-901903209</t>
         </is>
       </c>
     </row>
-    <row r="5" ht="25.5" customHeight="1">
-      <c r="A5" s="8" t="inlineStr">
+    <row r="5" ht="25.5" customHeight="1" s="123">
+      <c r="A5" s="127" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="B5" s="9" t="n"/>
-      <c r="C5" s="9" t="n"/>
-      <c r="D5" s="9" t="n"/>
-      <c r="E5" s="9" t="n"/>
-      <c r="F5" s="9" t="n"/>
-      <c r="G5" s="9" t="n"/>
-      <c r="H5" s="9" t="n"/>
-      <c r="I5" s="9" t="n"/>
-    </row>
-    <row r="6" ht="54" customHeight="1">
-      <c r="A6" s="10" t="inlineStr">
+      <c r="B5" s="128" t="n"/>
+      <c r="C5" s="128" t="n"/>
+      <c r="D5" s="128" t="n"/>
+      <c r="E5" s="128" t="n"/>
+      <c r="F5" s="128" t="n"/>
+      <c r="G5" s="128" t="n"/>
+      <c r="H5" s="128" t="n"/>
+      <c r="I5" s="128" t="n"/>
+    </row>
+    <row r="6" ht="54" customHeight="1" s="123">
+      <c r="A6" s="129" t="inlineStr">
         <is>
           <t>PACKING LIST</t>
         </is>
       </c>
-      <c r="B6" s="11" t="n"/>
-      <c r="C6" s="11" t="n"/>
-      <c r="D6" s="11" t="n"/>
-      <c r="E6" s="11" t="n"/>
-      <c r="F6" s="11" t="n"/>
-      <c r="G6" s="11" t="n"/>
-      <c r="H6" s="11" t="n"/>
-      <c r="I6" s="11" t="n"/>
-    </row>
-    <row r="7" ht="18" customHeight="1">
-      <c r="A7" s="12" t="n"/>
-      <c r="B7" s="13" t="n"/>
-      <c r="C7" s="12" t="n"/>
-      <c r="D7" s="12" t="n"/>
-      <c r="E7" s="6" t="n"/>
-      <c r="F7" s="6" t="n"/>
-      <c r="G7" s="6" t="n"/>
-      <c r="H7" s="14" t="inlineStr">
+      <c r="B6" s="130" t="n"/>
+      <c r="C6" s="130" t="n"/>
+      <c r="D6" s="130" t="n"/>
+      <c r="E6" s="130" t="n"/>
+      <c r="F6" s="130" t="n"/>
+      <c r="G6" s="130" t="n"/>
+      <c r="H6" s="130" t="n"/>
+      <c r="I6" s="130" t="n"/>
+    </row>
+    <row r="7" ht="18" customHeight="1" s="123">
+      <c r="A7" s="6" t="n"/>
+      <c r="B7" s="7" t="n"/>
+      <c r="C7" s="6" t="n"/>
+      <c r="D7" s="6" t="n"/>
+      <c r="E7" s="125" t="n"/>
+      <c r="F7" s="125" t="n"/>
+      <c r="G7" s="125" t="n"/>
+      <c r="H7" s="8" t="inlineStr">
         <is>
           <t>Ref No.:</t>
         </is>
       </c>
-      <c r="I7" s="62" t="inlineStr">
+      <c r="I7" s="52" t="inlineStr">
         <is>
           <t>JFREF</t>
         </is>
       </c>
     </row>
-    <row r="8" ht="30" customHeight="1">
-      <c r="A8" s="15" t="inlineStr">
+    <row r="8" ht="30" customHeight="1" s="123">
+      <c r="A8" s="9" t="inlineStr">
         <is>
           <t>EXPORTER:</t>
         </is>
       </c>
-      <c r="B8" s="16" t="inlineStr">
+      <c r="B8" s="10" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="F8" s="17" t="n"/>
-      <c r="G8" s="17" t="n"/>
-      <c r="H8" s="17" t="inlineStr">
+      <c r="F8" s="11" t="n"/>
+      <c r="G8" s="11" t="n"/>
+      <c r="H8" s="11" t="inlineStr">
         <is>
           <t>INVOICE NO :</t>
         </is>
       </c>
-      <c r="I8" s="63" t="inlineStr">
+      <c r="I8" s="53" t="inlineStr">
         <is>
           <t>JFINV</t>
         </is>
       </c>
     </row>
-    <row r="9" ht="21" customHeight="1">
-      <c r="A9" s="12" t="n"/>
-      <c r="B9" s="13" t="inlineStr">
+    <row r="9" ht="21" customHeight="1" s="123">
+      <c r="A9" s="6" t="n"/>
+      <c r="B9" s="7" t="inlineStr">
         <is>
           <t>XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages,</t>
         </is>
       </c>
-      <c r="F9" s="6" t="n"/>
-      <c r="G9" s="6" t="n"/>
-      <c r="H9" s="17" t="inlineStr">
+      <c r="F9" s="125" t="n"/>
+      <c r="G9" s="125" t="n"/>
+      <c r="H9" s="11" t="inlineStr">
         <is>
           <t>Date:</t>
         </is>
       </c>
-      <c r="I9" s="131" t="inlineStr">
+      <c r="I9" s="145" t="inlineStr">
         <is>
           <t>JFTIME</t>
         </is>
       </c>
     </row>
-    <row r="10" ht="22.5" customHeight="1">
-      <c r="A10" s="12" t="n"/>
-      <c r="B10" s="13" t="inlineStr">
+    <row r="10" ht="22.5" customHeight="1" s="123">
+      <c r="A10" s="6" t="n"/>
+      <c r="B10" s="7" t="inlineStr">
         <is>
           <t>Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia</t>
         </is>
       </c>
-      <c r="F10" s="6" t="n"/>
-      <c r="G10" s="6" t="n"/>
-      <c r="H10" s="18" t="inlineStr">
+      <c r="F10" s="125" t="n"/>
+      <c r="G10" s="125" t="n"/>
+      <c r="H10" s="12" t="inlineStr">
         <is>
           <t>FCA :</t>
         </is>
       </c>
-      <c r="I10" s="65" t="inlineStr">
+      <c r="I10" s="55" t="inlineStr">
         <is>
           <t>BAVET, SVAY RIENG</t>
         </is>
       </c>
     </row>
-    <row r="11" ht="20.25" customHeight="1">
-      <c r="A11" s="12" t="n"/>
-      <c r="B11" s="13" t="inlineStr">
+    <row r="11" ht="20.25" customHeight="1" s="123">
+      <c r="A11" s="6" t="n"/>
+      <c r="B11" s="7" t="inlineStr">
         <is>
           <t>Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="F11" s="6" t="n"/>
-      <c r="G11" s="6" t="n"/>
-      <c r="H11" s="6" t="n"/>
-      <c r="I11" s="6" t="n"/>
-    </row>
-    <row r="12" ht="15.75" customHeight="1">
-      <c r="A12" s="12" t="n"/>
-      <c r="B12" s="13" t="n"/>
-      <c r="C12" s="12" t="n"/>
-      <c r="D12" s="12" t="n"/>
-      <c r="E12" s="6" t="n"/>
-      <c r="F12" s="6" t="n"/>
-      <c r="G12" s="6" t="n"/>
-      <c r="H12" s="6" t="n"/>
-      <c r="I12" s="6" t="n"/>
-    </row>
-    <row r="13" ht="25.5" customHeight="1">
-      <c r="A13" s="19" t="inlineStr">
+      <c r="F11" s="125" t="n"/>
+      <c r="G11" s="125" t="n"/>
+      <c r="H11" s="125" t="n"/>
+      <c r="I11" s="125" t="n"/>
+    </row>
+    <row r="12" ht="15.75" customHeight="1" s="123">
+      <c r="A12" s="6" t="n"/>
+      <c r="B12" s="7" t="n"/>
+      <c r="C12" s="6" t="n"/>
+      <c r="D12" s="6" t="n"/>
+      <c r="E12" s="125" t="n"/>
+      <c r="F12" s="125" t="n"/>
+      <c r="G12" s="125" t="n"/>
+      <c r="H12" s="125" t="n"/>
+      <c r="I12" s="125" t="n"/>
+    </row>
+    <row r="13" ht="25.5" customHeight="1" s="123">
+      <c r="A13" s="13" t="inlineStr">
         <is>
           <t>CONSIGNEE :</t>
         </is>
       </c>
-      <c r="B13" s="20" t="inlineStr">
+      <c r="B13" s="14" t="inlineStr">
         <is>
           <t>JASON FURNITURE VIET NAM COMPANY LIMITED</t>
         </is>
       </c>
-      <c r="F13" s="21" t="n"/>
-      <c r="G13" s="21" t="n"/>
-      <c r="H13" s="21" t="n"/>
-      <c r="I13" s="27" t="n"/>
-    </row>
-    <row r="14" ht="25.5" customHeight="1">
-      <c r="A14" s="12" t="n"/>
-      <c r="B14" s="22" t="inlineStr">
+      <c r="F13" s="15" t="n"/>
+      <c r="G13" s="15" t="n"/>
+      <c r="H13" s="15" t="n"/>
+      <c r="I13" s="21" t="n"/>
+    </row>
+    <row r="14" ht="25.5" customHeight="1" s="123">
+      <c r="A14" s="6" t="n"/>
+      <c r="B14" s="16" t="inlineStr">
         <is>
           <t>LOT 37, 38, 39, 40, 41, 44, 50, 51, 54，55, 56，B2 CLUSTER, DONG XOAI III INDUSTRIAL ZONE,</t>
         </is>
       </c>
-      <c r="C14" s="23" t="n"/>
-      <c r="D14" s="23" t="n"/>
-      <c r="E14" s="24" t="n"/>
-      <c r="F14" s="24" t="n"/>
-      <c r="G14" s="24" t="n"/>
-      <c r="H14" s="24" t="n"/>
-    </row>
-    <row r="15" ht="21" customHeight="1">
-      <c r="A15" s="12" t="n"/>
-      <c r="B15" s="25" t="inlineStr">
+      <c r="C14" s="17" t="n"/>
+      <c r="D14" s="17" t="n"/>
+      <c r="E14" s="18" t="n"/>
+      <c r="F14" s="18" t="n"/>
+      <c r="G14" s="18" t="n"/>
+      <c r="H14" s="18" t="n"/>
+    </row>
+    <row r="15" ht="21" customHeight="1" s="123">
+      <c r="A15" s="6" t="n"/>
+      <c r="B15" s="19" t="inlineStr">
         <is>
           <t>BINH PHUOC WARD,DONG NAI PROVINCE, VIETNAM</t>
         </is>
       </c>
-      <c r="C15" s="26" t="n"/>
-      <c r="D15" s="26" t="n"/>
-      <c r="E15" s="27" t="n"/>
-      <c r="F15" s="27" t="n"/>
-      <c r="G15" s="27" t="n"/>
-      <c r="H15" s="27" t="n"/>
-    </row>
-    <row r="16" ht="21" customHeight="1">
-      <c r="A16" s="12" t="n"/>
-      <c r="B16" s="28" t="inlineStr">
+      <c r="C15" s="20" t="n"/>
+      <c r="D15" s="20" t="n"/>
+      <c r="E15" s="21" t="n"/>
+      <c r="F15" s="21" t="n"/>
+      <c r="G15" s="21" t="n"/>
+      <c r="H15" s="21" t="n"/>
+    </row>
+    <row r="16" ht="21" customHeight="1" s="123">
+      <c r="A16" s="6" t="n"/>
+      <c r="B16" s="22" t="inlineStr">
         <is>
           <t>Contact Person : Mr. Thuy   TEl: 0379367084</t>
         </is>
       </c>
-      <c r="C16" s="26" t="n"/>
-      <c r="D16" s="26" t="n"/>
-      <c r="E16" s="27" t="n"/>
-      <c r="F16" s="27" t="n"/>
-      <c r="G16" s="27" t="n"/>
-      <c r="H16" s="27" t="n"/>
-    </row>
-    <row r="17" ht="21" customHeight="1">
-      <c r="A17" s="12" t="n"/>
-      <c r="B17" s="28" t="inlineStr">
+      <c r="C16" s="20" t="n"/>
+      <c r="D16" s="20" t="n"/>
+      <c r="E16" s="21" t="n"/>
+      <c r="F16" s="21" t="n"/>
+      <c r="G16" s="21" t="n"/>
+      <c r="H16" s="21" t="n"/>
+    </row>
+    <row r="17" ht="21" customHeight="1" s="123">
+      <c r="A17" s="6" t="n"/>
+      <c r="B17" s="22" t="inlineStr">
         <is>
           <t>EMAlL:jyangbin4720@dingtalk.com jialy@kukahome.com</t>
         </is>
       </c>
-      <c r="C17" s="26" t="n"/>
-      <c r="D17" s="26" t="n"/>
-      <c r="E17" s="27" t="n"/>
-      <c r="F17" s="27" t="n"/>
-      <c r="G17" s="27" t="n"/>
-      <c r="H17" s="27" t="n"/>
-    </row>
-    <row r="18" ht="21" customHeight="1">
-      <c r="A18" s="12" t="n"/>
-      <c r="B18" s="28" t="inlineStr">
+      <c r="C17" s="20" t="n"/>
+      <c r="D17" s="20" t="n"/>
+      <c r="E17" s="21" t="n"/>
+      <c r="F17" s="21" t="n"/>
+      <c r="G17" s="21" t="n"/>
+      <c r="H17" s="21" t="n"/>
+    </row>
+    <row r="18" ht="21" customHeight="1" s="123">
+      <c r="A18" s="6" t="n"/>
+      <c r="B18" s="22" t="inlineStr">
         <is>
           <t>dailin@kukahome.com huanggf@kukahome.com zhangzp@kukahome.com</t>
         </is>
       </c>
-      <c r="C18" s="12" t="n"/>
-      <c r="D18" s="12" t="n"/>
-      <c r="E18" s="6" t="n"/>
-      <c r="F18" s="6" t="n"/>
-      <c r="G18" s="6" t="n"/>
-      <c r="H18" s="6" t="n"/>
-    </row>
-    <row r="19" ht="27.75" customHeight="1">
-      <c r="A19" s="29" t="inlineStr">
+      <c r="C18" s="6" t="n"/>
+      <c r="D18" s="6" t="n"/>
+      <c r="E18" s="125" t="n"/>
+      <c r="F18" s="125" t="n"/>
+      <c r="G18" s="125" t="n"/>
+      <c r="H18" s="125" t="n"/>
+    </row>
+    <row r="19" ht="27.75" customHeight="1" s="123">
+      <c r="A19" s="23" t="inlineStr">
         <is>
           <t xml:space="preserve">SHIP: </t>
         </is>
       </c>
-      <c r="B19" s="13" t="inlineStr">
+      <c r="B19" s="7" t="inlineStr">
         <is>
           <t>BY TRUCK FROM BAVET, SVAY RIENG, CAMBODIA TO DONG NAI PROVINCE, VIETNAM.</t>
         </is>
       </c>
     </row>
-    <row r="20" ht="27.75" customHeight="1">
-      <c r="A20" s="30" t="n"/>
-      <c r="B20" s="31" t="n"/>
-    </row>
-    <row r="21" ht="27" customHeight="1"/>
-    <row r="22" ht="27" customHeight="1"/>
-    <row r="23" ht="27" customHeight="1"/>
-    <row r="24" ht="27" customHeight="1">
-      <c r="A24" s="30" t="n"/>
-      <c r="B24" s="31" t="n"/>
-    </row>
-    <row r="25" ht="27" customHeight="1">
-      <c r="A25" s="45" t="inlineStr">
+    <row r="20" ht="27.75" customHeight="1" s="123">
+      <c r="A20" s="24" t="n"/>
+      <c r="B20" s="25" t="n"/>
+    </row>
+    <row r="21" ht="27" customHeight="1" s="123"/>
+    <row r="22" ht="27" customHeight="1" s="123"/>
+    <row r="23" ht="27" customHeight="1" s="123"/>
+    <row r="24" ht="27" customHeight="1" s="123">
+      <c r="A24" s="24" t="n"/>
+      <c r="B24" s="25" t="n"/>
+    </row>
+    <row r="25" ht="27" customHeight="1" s="123">
+      <c r="A25" s="36" t="inlineStr">
         <is>
           <t>Country of Original Cambodia</t>
         </is>
       </c>
-      <c r="B25" s="45" t="n"/>
-      <c r="C25" s="45" t="n"/>
-      <c r="D25" s="46" t="n"/>
-      <c r="E25" s="47" t="n"/>
-      <c r="F25" s="6" t="n"/>
-      <c r="G25" s="6" t="n"/>
-      <c r="H25" s="6" t="n"/>
-    </row>
-    <row r="26" ht="65.25" customHeight="1">
-      <c r="A26" s="48" t="inlineStr">
+      <c r="B25" s="36" t="n"/>
+      <c r="C25" s="36" t="n"/>
+      <c r="D25" s="131" t="n"/>
+      <c r="E25" s="38" t="n"/>
+      <c r="F25" s="125" t="n"/>
+      <c r="G25" s="125" t="n"/>
+      <c r="H25" s="125" t="n"/>
+    </row>
+    <row r="26" ht="65.25" customHeight="1" s="123">
+      <c r="A26" s="39" t="inlineStr">
         <is>
           <t>Manufacture:</t>
         </is>
       </c>
-      <c r="B26" s="49" t="inlineStr">
+      <c r="B26" s="140" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.
 XIN BAVET SEZ, Road No. 316A, Trapeang Bon and Prey Kokir Villages, Prey Kokir Commune, Chantrea District,Svay Rieng Province, Kingdom of Cambodia, Tel: +855   975910636</t>
         </is>
       </c>
-      <c r="E26" s="50" t="n"/>
-      <c r="F26" s="50" t="n"/>
-      <c r="G26" s="50" t="n"/>
-      <c r="H26" s="6" t="n"/>
-    </row>
-    <row r="27" ht="51.75" customHeight="1">
-      <c r="A27" s="49" t="inlineStr">
+      <c r="E26" s="40" t="n"/>
+      <c r="F26" s="40" t="n"/>
+      <c r="G26" s="40" t="n"/>
+      <c r="H26" s="125" t="n"/>
+    </row>
+    <row r="27" ht="51.75" customHeight="1" s="123">
+      <c r="A27" s="140" t="inlineStr">
         <is>
           <t>BENEFICIARY BANK：BANK OF CHINA(HONG KONG)LIMITED  PHNOM PENH BRANCH
                                           /BANK OF CHINA PHNOM PENH BRANCH</t>
         </is>
       </c>
-      <c r="E27" s="50" t="n"/>
-      <c r="F27" s="50" t="n"/>
-      <c r="G27" s="50" t="n"/>
-      <c r="H27" s="50" t="n"/>
-    </row>
-    <row r="28" ht="27" customHeight="1">
-      <c r="A28" s="51" t="inlineStr">
+      <c r="E27" s="40" t="n"/>
+      <c r="F27" s="40" t="n"/>
+      <c r="G27" s="40" t="n"/>
+      <c r="H27" s="40" t="n"/>
+    </row>
+    <row r="28" ht="27" customHeight="1" s="123">
+      <c r="A28" s="134" t="inlineStr">
         <is>
           <t>A/C NO:100001100764430</t>
         </is>
       </c>
-      <c r="B28" s="51" t="n"/>
-      <c r="C28" s="51" t="n"/>
-      <c r="D28" s="51" t="n"/>
-      <c r="E28" s="52" t="n"/>
-      <c r="F28" s="52" t="n"/>
-      <c r="G28" s="52" t="n"/>
-      <c r="H28" s="52" t="n"/>
-    </row>
-    <row r="29" ht="27" customHeight="1">
-      <c r="A29" s="51" t="inlineStr">
+      <c r="B28" s="134" t="n"/>
+      <c r="C28" s="134" t="n"/>
+      <c r="D28" s="134" t="n"/>
+      <c r="E28" s="42" t="n"/>
+      <c r="F28" s="42" t="n"/>
+      <c r="G28" s="42" t="n"/>
+      <c r="H28" s="42" t="n"/>
+    </row>
+    <row r="29" ht="27" customHeight="1" s="123">
+      <c r="A29" s="134" t="inlineStr">
         <is>
           <t>SWIFT CODE  ：BKCHKHPPXXX</t>
         </is>
       </c>
-      <c r="B29" s="51" t="n"/>
-      <c r="C29" s="51" t="n"/>
-      <c r="D29" s="51" t="n"/>
-      <c r="E29" s="52" t="n"/>
-      <c r="F29" s="52" t="n"/>
-      <c r="G29" s="52" t="n"/>
-      <c r="H29" s="52" t="n"/>
-    </row>
-    <row r="30" ht="27" customHeight="1">
-      <c r="A30" s="53" t="n"/>
-      <c r="B30" s="54" t="n"/>
-      <c r="C30" s="53" t="n"/>
-      <c r="D30" s="53" t="n"/>
-      <c r="E30" s="55" t="n"/>
-      <c r="G30" s="6" t="inlineStr">
+      <c r="B29" s="134" t="n"/>
+      <c r="C29" s="134" t="n"/>
+      <c r="D29" s="134" t="n"/>
+      <c r="E29" s="42" t="n"/>
+      <c r="F29" s="42" t="n"/>
+      <c r="G29" s="42" t="n"/>
+      <c r="H29" s="42" t="n"/>
+    </row>
+    <row r="30" ht="27" customHeight="1" s="123">
+      <c r="A30" s="43" t="n"/>
+      <c r="B30" s="44" t="n"/>
+      <c r="C30" s="43" t="n"/>
+      <c r="D30" s="43" t="n"/>
+      <c r="E30" s="45" t="n"/>
+      <c r="G30" s="125" t="inlineStr">
         <is>
           <t>CALIFOR UPHOLSTERY MATERIALS CO., LTD.</t>
         </is>
       </c>
-      <c r="H30" s="55" t="n"/>
-    </row>
-    <row r="31" ht="27" customHeight="1"/>
-    <row r="32" ht="27" customHeight="1"/>
-    <row r="33" ht="27" customHeight="1"/>
-    <row r="34" ht="27" customHeight="1"/>
-    <row r="35" ht="27" customHeight="1"/>
+      <c r="H30" s="45" t="n"/>
+    </row>
+    <row r="31" ht="27" customHeight="1" s="123"/>
+    <row r="32" ht="27" customHeight="1" s="123"/>
+    <row r="33" ht="27" customHeight="1" s="123"/>
+    <row r="34" ht="27" customHeight="1" s="123"/>
+    <row r="35" ht="27" customHeight="1" s="123"/>
     <row r="36" ht="27" customFormat="1" customHeight="1" s="1"/>
-    <row r="37" ht="27" customHeight="1"/>
-    <row r="38" ht="27" customHeight="1"/>
-    <row r="39" ht="21" customHeight="1"/>
-    <row r="40" ht="21" customHeight="1"/>
-    <row r="41" ht="65.25" customHeight="1"/>
-    <row r="42" ht="51.75" customHeight="1"/>
-    <row r="43" ht="21" customHeight="1"/>
-    <row r="44" ht="17.25" customHeight="1"/>
+    <row r="37" ht="27" customHeight="1" s="123"/>
+    <row r="38" ht="27" customHeight="1" s="123"/>
+    <row r="39" ht="21" customHeight="1" s="123"/>
+    <row r="40" ht="21" customHeight="1" s="123"/>
+    <row r="41" ht="65.25" customHeight="1" s="123"/>
+    <row r="42" ht="51.75" customHeight="1" s="123"/>
+    <row r="43" ht="21" customHeight="1" s="123"/>
+    <row r="44" ht="17.25" customHeight="1" s="123"/>
     <row r="45"/>
     <row r="46"/>
     <row r="47"/>
@@ -3600,18 +3027,18 @@
     <row r="53"/>
     <row r="54"/>
     <row r="55"/>
-    <row r="56"/>
+    <row r="56" ht="15" customHeight="1" s="123"/>
     <row r="57"/>
-    <row r="58" ht="16.5" customHeight="1"/>
-    <row r="59" ht="16.5" customHeight="1"/>
-    <row r="60" ht="16.5" customHeight="1"/>
-    <row r="61" ht="16.5" customHeight="1"/>
-    <row r="62" ht="16.5" customHeight="1"/>
-    <row r="63" ht="16.5" customHeight="1"/>
-    <row r="64" ht="115.65" customHeight="1"/>
-    <row r="65" ht="113.7" customHeight="1"/>
-    <row r="66" ht="16.5" customHeight="1"/>
-    <row r="67" ht="16.5" customHeight="1"/>
+    <row r="58" ht="15.6" customHeight="1" s="123"/>
+    <row r="59" ht="15.6" customHeight="1" s="123"/>
+    <row r="60" ht="15.6" customHeight="1" s="123"/>
+    <row r="61" ht="15.6" customHeight="1" s="123"/>
+    <row r="62" ht="15.6" customHeight="1" s="123"/>
+    <row r="63" ht="15.6" customHeight="1" s="123"/>
+    <row r="64" ht="115.65" customHeight="1" s="123"/>
+    <row r="65" ht="113.7" customHeight="1" s="123"/>
+    <row r="66" ht="15.6" customHeight="1" s="123"/>
+    <row r="67" ht="16.8" customHeight="1" s="123"/>
     <row r="68"/>
     <row r="69"/>
     <row r="70"/>
@@ -3748,15 +3175,15 @@
   </sheetData>
   <mergeCells count="10">
     <mergeCell ref="B41:D41"/>
+    <mergeCell ref="A4:I4"/>
     <mergeCell ref="B26:D26"/>
     <mergeCell ref="A3:I3"/>
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A42:D42"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="A1:I1"/>
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A4:I4"/>
+    <mergeCell ref="A42:D42"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.314583333333333" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
the row shift merge after row delete is now fixing by removing the merge property at the range of the deletion and also the range of cell below going to shift to preventing currupt merge
</commit_message>
<xml_diff>
--- a/invoice_gen/TEMPLATE/JF.xlsx
+++ b/invoice_gen/TEMPLATE/JF.xlsx
@@ -1973,18 +1973,14 @@
     <row r="199"/>
     <row r="200" ht="27.9" customHeight="1" s="123"/>
   </sheetData>
-  <mergeCells count="13">
-    <mergeCell ref="C28:E28"/>
-    <mergeCell ref="C27:E27"/>
+  <mergeCells count="9">
     <mergeCell ref="A200:B200"/>
     <mergeCell ref="C23:E23"/>
     <mergeCell ref="C22:E22"/>
     <mergeCell ref="A1:E1"/>
-    <mergeCell ref="C26:E26"/>
-    <mergeCell ref="B11:E11"/>
     <mergeCell ref="A13:E13"/>
     <mergeCell ref="A14:E14"/>
-    <mergeCell ref="A189:B189"/>
+    <mergeCell ref="B11:E11"/>
     <mergeCell ref="B10:E10"/>
     <mergeCell ref="C24:E24"/>
   </mergeCells>
@@ -2590,18 +2586,14 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="A32:G32"/>
+  <mergeCells count="11">
     <mergeCell ref="A1:G1"/>
-    <mergeCell ref="B29:C29"/>
     <mergeCell ref="B25:C25"/>
-    <mergeCell ref="A31:G31"/>
+    <mergeCell ref="A27:G27"/>
     <mergeCell ref="A3:G3"/>
     <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A27:G27"/>
     <mergeCell ref="A4:G4"/>
     <mergeCell ref="A2:G2"/>
-    <mergeCell ref="A30:C30"/>
     <mergeCell ref="A28:G28"/>
     <mergeCell ref="A26:C26"/>
     <mergeCell ref="A24:C24"/>
@@ -3173,17 +3165,15 @@
     <row r="199"/>
     <row r="200"/>
   </sheetData>
-  <mergeCells count="10">
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="A4:I4"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="A3:I3"/>
+  <mergeCells count="8">
     <mergeCell ref="A27:D27"/>
     <mergeCell ref="A2:I2"/>
     <mergeCell ref="A5:I5"/>
     <mergeCell ref="A1:I1"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="A3:I3"/>
     <mergeCell ref="A6:I6"/>
-    <mergeCell ref="A42:D42"/>
+    <mergeCell ref="A4:I4"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.314583333333333" bottom="0" header="0" footer="0"/>

</xml_diff>